<commit_message>
SET 1 [0..5] Single
</commit_message>
<xml_diff>
--- a/RESULTS/SET 1 [0..5] Single/050.0%/BE.xlsx
+++ b/RESULTS/SET 1 [0..5] Single/050.0%/BE.xlsx
@@ -17,9 +17,6 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="7" sheetId="9" state="visible" r:id="rId9"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="6" sheetId="10" state="visible" r:id="rId10"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="5" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="4" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="3" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2" sheetId="14" state="visible" r:id="rId14"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -27,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="76">
   <si>
     <t>Feature index</t>
   </si>
@@ -110,10 +107,67 @@
     <t>001111</t>
   </si>
   <si>
-    <t>031155</t>
-  </si>
-  <si>
-    <t>003111</t>
+    <t>010055</t>
+  </si>
+  <si>
+    <t>O-O</t>
+  </si>
+  <si>
+    <t>001100</t>
+  </si>
+  <si>
+    <t>150055</t>
+  </si>
+  <si>
+    <t>015100</t>
+  </si>
+  <si>
+    <t>110055</t>
+  </si>
+  <si>
+    <t>011100</t>
+  </si>
+  <si>
+    <t>151155</t>
+  </si>
+  <si>
+    <t>015111</t>
+  </si>
+  <si>
+    <t>141155</t>
+  </si>
+  <si>
+    <t>014111</t>
+  </si>
+  <si>
+    <t>131155</t>
+  </si>
+  <si>
+    <t>013111</t>
+  </si>
+  <si>
+    <t>090055</t>
+  </si>
+  <si>
+    <t>009100</t>
+  </si>
+  <si>
+    <t>121155</t>
+  </si>
+  <si>
+    <t>012111</t>
+  </si>
+  <si>
+    <t>111155</t>
+  </si>
+  <si>
+    <t>011111</t>
+  </si>
+  <si>
+    <t>070055</t>
+  </si>
+  <si>
+    <t>007100</t>
   </si>
   <si>
     <t>051155</t>
@@ -122,43 +176,46 @@
     <t>005111</t>
   </si>
   <si>
-    <t>071155</t>
-  </si>
-  <si>
-    <t>007111</t>
-  </si>
-  <si>
-    <t>111155</t>
-  </si>
-  <si>
-    <t>011111</t>
-  </si>
-  <si>
-    <t>121155</t>
-  </si>
-  <si>
-    <t>012111</t>
-  </si>
-  <si>
-    <t>090055</t>
-  </si>
-  <si>
-    <t>O-O</t>
-  </si>
-  <si>
-    <t>009100</t>
-  </si>
-  <si>
-    <t>100055</t>
-  </si>
-  <si>
-    <t>010100</t>
-  </si>
-  <si>
-    <t>110055</t>
-  </si>
-  <si>
-    <t>011100</t>
+    <t>100155</t>
+  </si>
+  <si>
+    <t>010101</t>
+  </si>
+  <si>
+    <t>090155</t>
+  </si>
+  <si>
+    <t>009101</t>
+  </si>
+  <si>
+    <t>101155</t>
+  </si>
+  <si>
+    <t>010111</t>
+  </si>
+  <si>
+    <t>091155</t>
+  </si>
+  <si>
+    <t>009111</t>
+  </si>
+  <si>
+    <t>140055</t>
+  </si>
+  <si>
+    <t>014100</t>
+  </si>
+  <si>
+    <t>080055</t>
+  </si>
+  <si>
+    <t>008100</t>
+  </si>
+  <si>
+    <t>150155</t>
+  </si>
+  <si>
+    <t>015101</t>
   </si>
   <si>
     <t>120055</t>
@@ -167,100 +224,34 @@
     <t>012100</t>
   </si>
   <si>
+    <t>060055</t>
+  </si>
+  <si>
+    <t>006100</t>
+  </si>
+  <si>
+    <t>050055</t>
+  </si>
+  <si>
+    <t>005100</t>
+  </si>
+  <si>
     <t>130055</t>
   </si>
   <si>
     <t>013100</t>
   </si>
   <si>
-    <t>140055</t>
-  </si>
-  <si>
-    <t>014100</t>
-  </si>
-  <si>
-    <t>150055</t>
-  </si>
-  <si>
-    <t>015100</t>
-  </si>
-  <si>
-    <t>150155</t>
-  </si>
-  <si>
-    <t>015101</t>
-  </si>
-  <si>
-    <t>040055</t>
-  </si>
-  <si>
-    <t>004100</t>
-  </si>
-  <si>
-    <t>080055</t>
-  </si>
-  <si>
-    <t>008100</t>
-  </si>
-  <si>
-    <t>141155</t>
-  </si>
-  <si>
-    <t>014111</t>
-  </si>
-  <si>
-    <t>131155</t>
-  </si>
-  <si>
-    <t>013111</t>
-  </si>
-  <si>
-    <t>151155</t>
-  </si>
-  <si>
-    <t>015111</t>
-  </si>
-  <si>
-    <t>021155</t>
-  </si>
-  <si>
-    <t>002111</t>
-  </si>
-  <si>
-    <t>070055</t>
-  </si>
-  <si>
-    <t>007100</t>
-  </si>
-  <si>
-    <t>010055</t>
-  </si>
-  <si>
-    <t>001100</t>
-  </si>
-  <si>
-    <t>060055</t>
-  </si>
-  <si>
-    <t>006100</t>
+    <t>130155</t>
+  </si>
+  <si>
+    <t>013101</t>
   </si>
   <si>
     <t>081155</t>
   </si>
   <si>
     <t>008111</t>
-  </si>
-  <si>
-    <t>101155</t>
-  </si>
-  <si>
-    <t>010111</t>
-  </si>
-  <si>
-    <t>020155</t>
-  </si>
-  <si>
-    <t>002101</t>
   </si>
 </sst>
 </file>
@@ -708,27 +699,27 @@
         <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.1220997564137293</v>
+        <v>-0.1199619968253992</v>
       </c>
       <c r="K2" t="s"/>
       <c r="L2" t="n">
-        <v>4.001079082411344e-07</v>
+        <v>3.44324027811439e-07</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0006325408352360616</v>
+        <v>0.0005867912983433198</v>
       </c>
       <c r="N2" t="n">
-        <v>0.9137846606912122</v>
+        <v>0.9273450391945901</v>
       </c>
       <c r="O2" t="n">
-        <v>0.909912714315069</v>
+        <v>0.9240820918530298</v>
       </c>
       <c r="P2" t="s"/>
       <c r="Q2" t="s"/>
       <c r="R2" t="s"/>
       <c r="S2" t="s"/>
       <c r="T2" t="n">
-        <v>72.72163444099954</v>
+        <v>51.77003994762144</v>
       </c>
       <c r="U2" t="s"/>
     </row>
@@ -761,7 +752,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="n">
-        <v>0.1313828107149392</v>
+        <v>0.07408974723730793</v>
       </c>
       <c r="K3" t="s"/>
       <c r="L3" t="s"/>
@@ -780,31 +771,31 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
         <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E4" t="n">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="F4" t="s">
         <v>22</v>
       </c>
       <c r="G4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I4" t="n">
         <v>1</v>
       </c>
       <c r="J4" t="n">
-        <v>-1.149783575552945</v>
+        <v>0.1884144077928456</v>
       </c>
       <c r="K4" t="s"/>
       <c r="L4" t="s"/>
@@ -823,31 +814,31 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E5" t="n">
-        <v>-5</v>
+        <v>-15</v>
       </c>
       <c r="F5" t="s">
         <v>22</v>
       </c>
       <c r="G5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H5" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I5" t="n">
         <v>1</v>
       </c>
       <c r="J5" t="n">
-        <v>11.09684660040507</v>
+        <v>-381339.5799724752</v>
       </c>
       <c r="K5" t="s"/>
       <c r="L5" t="s"/>
@@ -866,31 +857,31 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E6" t="n">
-        <v>-7</v>
+        <v>-11</v>
       </c>
       <c r="F6" t="s">
         <v>22</v>
       </c>
       <c r="G6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H6" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I6" t="n">
         <v>1</v>
       </c>
       <c r="J6" t="n">
-        <v>-46.65887747498497</v>
+        <v>35962.12871283893</v>
       </c>
       <c r="K6" t="s"/>
       <c r="L6" t="s"/>
@@ -909,22 +900,22 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
         <v>25</v>
       </c>
       <c r="E7" t="n">
-        <v>-11</v>
+        <v>-15</v>
       </c>
       <c r="F7" t="s">
         <v>22</v>
       </c>
       <c r="G7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H7" t="n">
         <v>4</v>
@@ -933,7 +924,7 @@
         <v>1</v>
       </c>
       <c r="J7" t="n">
-        <v>762.6878441862839</v>
+        <v>471452.2383175354</v>
       </c>
       <c r="K7" t="s"/>
       <c r="L7" t="s"/>
@@ -952,22 +943,22 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
         <v>25</v>
       </c>
       <c r="E8" t="n">
-        <v>-12</v>
+        <v>-14</v>
       </c>
       <c r="F8" t="s">
         <v>22</v>
       </c>
       <c r="G8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H8" t="n">
         <v>4</v>
@@ -976,7 +967,7 @@
         <v>1</v>
       </c>
       <c r="J8" t="n">
-        <v>-978.5106257978139</v>
+        <v>-990127.7523702133</v>
       </c>
       <c r="K8" t="s"/>
       <c r="L8" t="s"/>
@@ -995,16 +986,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="E9" t="n">
-        <v>-9</v>
+        <v>-13</v>
       </c>
       <c r="F9" t="s">
         <v>22</v>
@@ -1013,13 +1004,13 @@
         <v>39</v>
       </c>
       <c r="H9" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>4803026.420101855</v>
+        <v>786157.4974569512</v>
       </c>
       <c r="K9" t="s"/>
       <c r="L9" t="s"/>
@@ -1038,16 +1029,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
         <v>40</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E10" t="n">
-        <v>-10</v>
+        <v>-9</v>
       </c>
       <c r="F10" t="s">
         <v>22</v>
@@ -1062,7 +1053,7 @@
         <v>1</v>
       </c>
       <c r="J10" t="n">
-        <v>-86079476.43453687</v>
+        <v>-6119.982451688734</v>
       </c>
       <c r="K10" t="s"/>
       <c r="L10" t="s"/>
@@ -1081,16 +1072,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
         <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="E11" t="n">
-        <v>-11</v>
+        <v>-12</v>
       </c>
       <c r="F11" t="s">
         <v>22</v>
@@ -1099,13 +1090,13 @@
         <v>43</v>
       </c>
       <c r="H11" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I11" t="n">
         <v>1</v>
       </c>
       <c r="J11" t="n">
-        <v>649712897.1352004</v>
+        <v>-280807.7225495961</v>
       </c>
       <c r="K11" t="s"/>
       <c r="L11" t="s"/>
@@ -1124,16 +1115,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
         <v>44</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="E12" t="n">
-        <v>-12</v>
+        <v>-11</v>
       </c>
       <c r="F12" t="s">
         <v>22</v>
@@ -1142,13 +1133,13 @@
         <v>45</v>
       </c>
       <c r="H12" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I12" t="n">
         <v>1</v>
       </c>
       <c r="J12" t="n">
-        <v>-2633422769.344817</v>
+        <v>38301.73217641743</v>
       </c>
       <c r="K12" t="s"/>
       <c r="L12" t="s"/>
@@ -1167,16 +1158,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
         <v>46</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E13" t="n">
-        <v>-13</v>
+        <v>-7</v>
       </c>
       <c r="F13" t="s">
         <v>22</v>
@@ -1191,7 +1182,7 @@
         <v>1</v>
       </c>
       <c r="J13" t="n">
-        <v>6028596306.236825</v>
+        <v>315.1824536681524</v>
       </c>
       <c r="K13" t="s"/>
       <c r="L13" t="s"/>
@@ -1210,16 +1201,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
         <v>48</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="E14" t="n">
-        <v>-14</v>
+        <v>-5</v>
       </c>
       <c r="F14" t="s">
         <v>22</v>
@@ -1228,13 +1219,13 @@
         <v>49</v>
       </c>
       <c r="H14" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I14" t="n">
         <v>1</v>
       </c>
       <c r="J14" t="n">
-        <v>-7375771590.260799</v>
+        <v>-2.286584842484444</v>
       </c>
       <c r="K14" t="s"/>
       <c r="L14" t="s"/>
@@ -1253,16 +1244,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
         <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="E15" t="n">
-        <v>-15</v>
+        <v>-10</v>
       </c>
       <c r="F15" t="s">
         <v>22</v>
@@ -1271,13 +1262,13 @@
         <v>51</v>
       </c>
       <c r="H15" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I15" t="n">
         <v>1</v>
       </c>
       <c r="J15" t="n">
-        <v>3762232290.954269</v>
+        <v>7.931181086692959</v>
       </c>
       <c r="K15" t="s"/>
       <c r="L15" t="s"/>
@@ -1296,7 +1287,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
         <v>52</v>
@@ -1305,7 +1296,7 @@
         <v>21</v>
       </c>
       <c r="E16" t="n">
-        <v>-15</v>
+        <v>-9</v>
       </c>
       <c r="F16" t="s">
         <v>22</v>
@@ -1320,7 +1311,7 @@
         <v>1</v>
       </c>
       <c r="J16" t="n">
-        <v>1.532100185751915</v>
+        <v>-4.753538885619491</v>
       </c>
       <c r="K16" t="s"/>
       <c r="L16" t="s"/>
@@ -1444,27 +1435,27 @@
         <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>0.06349489578538939</v>
+        <v>0.06301302159069891</v>
       </c>
       <c r="K2" t="s"/>
       <c r="L2" t="n">
-        <v>4.682916915699338e-07</v>
+        <v>4.290438330793451e-07</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0006843184138761238</v>
+        <v>0.0006550143762386785</v>
       </c>
       <c r="N2" t="n">
-        <v>0.8990924041924817</v>
+        <v>0.9094685227914058</v>
       </c>
       <c r="O2" t="n">
-        <v>0.8973272567439536</v>
+        <v>0.9078848817906724</v>
       </c>
       <c r="P2" t="s"/>
       <c r="Q2" t="s"/>
       <c r="R2" t="s"/>
       <c r="S2" t="s"/>
       <c r="T2" t="n">
-        <v>133.9954143402896</v>
+        <v>137.6881773053224</v>
       </c>
       <c r="U2" t="s"/>
     </row>
@@ -1497,7 +1488,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="n">
-        <v>-0.1234900961495514</v>
+        <v>-0.1230108232858482</v>
       </c>
       <c r="K3" t="s"/>
       <c r="L3" t="s"/>
@@ -1519,10 +1510,10 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E4" t="n">
         <v>-1</v>
@@ -1531,7 +1522,7 @@
         <v>22</v>
       </c>
       <c r="G4" t="s">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="H4" t="n">
         <v>1</v>
@@ -1540,7 +1531,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="n">
-        <v>0.2409258726454332</v>
+        <v>0.241319520986244</v>
       </c>
       <c r="K4" t="s"/>
       <c r="L4" t="s"/>
@@ -1562,10 +1553,10 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E5" t="n">
         <v>-15</v>
@@ -1574,7 +1565,7 @@
         <v>22</v>
       </c>
       <c r="G5" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="H5" t="n">
         <v>1</v>
@@ -1583,7 +1574,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="n">
-        <v>18703.32868635896</v>
+        <v>16706.5406171403</v>
       </c>
       <c r="K5" t="s"/>
       <c r="L5" t="s"/>
@@ -1605,7 +1596,7 @@
         <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="D6" t="s">
         <v>25</v>
@@ -1617,7 +1608,7 @@
         <v>22</v>
       </c>
       <c r="G6" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="H6" t="n">
         <v>4</v>
@@ -1626,7 +1617,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.1216682832896847</v>
+        <v>-0.1505495973870638</v>
       </c>
       <c r="K6" t="s"/>
       <c r="L6" t="s"/>
@@ -1645,7 +1636,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
         <v>74</v>
@@ -1654,7 +1645,7 @@
         <v>25</v>
       </c>
       <c r="E7" t="n">
-        <v>-10</v>
+        <v>-8</v>
       </c>
       <c r="F7" t="s">
         <v>22</v>
@@ -1669,7 +1660,7 @@
         <v>1</v>
       </c>
       <c r="J7" t="n">
-        <v>2.226406419201584</v>
+        <v>0.9114468826360733</v>
       </c>
       <c r="K7" t="s"/>
       <c r="L7" t="s"/>
@@ -1793,27 +1784,27 @@
         <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.1200397483765346</v>
+        <v>-0.1196876757647358</v>
       </c>
       <c r="K2" t="s"/>
       <c r="L2" t="n">
-        <v>4.935710175670431e-07</v>
+        <v>4.695832300493091e-07</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0007025460964001175</v>
+        <v>0.0006852614318997598</v>
       </c>
       <c r="N2" t="n">
-        <v>0.8936452095146281</v>
+        <v>0.9009144049836859</v>
       </c>
       <c r="O2" t="n">
-        <v>0.8920993550017593</v>
+        <v>0.8994742073817046</v>
       </c>
       <c r="P2" t="s"/>
       <c r="Q2" t="s"/>
       <c r="R2" t="s"/>
       <c r="S2" t="s"/>
       <c r="T2" t="n">
-        <v>158.9208220411195</v>
+        <v>182.1483680870013</v>
       </c>
       <c r="U2" t="s"/>
     </row>
@@ -1846,7 +1837,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="n">
-        <v>0.05870949551683649</v>
+        <v>0.05828112125975875</v>
       </c>
       <c r="K3" t="s"/>
       <c r="L3" t="s"/>
@@ -1868,10 +1859,10 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E4" t="n">
         <v>-1</v>
@@ -1880,7 +1871,7 @@
         <v>22</v>
       </c>
       <c r="G4" t="s">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="H4" t="n">
         <v>1</v>
@@ -1889,7 +1880,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="n">
-        <v>0.2456871670480333</v>
+        <v>0.2458744694270632</v>
       </c>
       <c r="K4" t="s"/>
       <c r="L4" t="s"/>
@@ -1908,22 +1899,22 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E5" t="n">
-        <v>-10</v>
+        <v>-13</v>
       </c>
       <c r="F5" t="s">
         <v>22</v>
       </c>
       <c r="G5" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="H5" t="n">
         <v>1</v>
@@ -1932,7 +1923,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="n">
-        <v>1147.396837103258</v>
+        <v>4039.933733089914</v>
       </c>
       <c r="K5" t="s"/>
       <c r="L5" t="s"/>
@@ -1951,22 +1942,22 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E6" t="n">
-        <v>-9</v>
+        <v>-7</v>
       </c>
       <c r="F6" t="s">
         <v>22</v>
       </c>
       <c r="G6" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="H6" t="n">
         <v>1</v>
@@ -1975,7 +1966,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="n">
-        <v>-400.3364919499872</v>
+        <v>-7.154232848370739</v>
       </c>
       <c r="K6" t="s"/>
       <c r="L6" t="s"/>
@@ -1988,666 +1979,6 @@
       <c r="S6" t="s"/>
       <c r="T6" t="s"/>
       <c r="U6" t="s"/>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:U5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:21">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" t="n">
-        <v>-1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" t="n">
-        <v>4</v>
-      </c>
-      <c r="I2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" t="n">
-        <v>-0.1331435359803878</v>
-      </c>
-      <c r="K2" t="s"/>
-      <c r="L2" t="n">
-        <v>6.262227560795236e-07</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0.000791342376016553</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0.8650613839760898</v>
-      </c>
-      <c r="O2" t="n">
-        <v>0.863496878283059</v>
-      </c>
-      <c r="P2" t="s"/>
-      <c r="Q2" t="s"/>
-      <c r="R2" t="s"/>
-      <c r="S2" t="s"/>
-      <c r="T2" t="n">
-        <v>292.8451822453696</v>
-      </c>
-      <c r="U2" t="s"/>
-    </row>
-    <row r="3" spans="1:21">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>30</v>
-      </c>
-      <c r="C3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" t="n">
-        <v>-1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" t="n">
-        <v>4</v>
-      </c>
-      <c r="I3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.06528372606195132</v>
-      </c>
-      <c r="K3" t="s"/>
-      <c r="L3" t="s"/>
-      <c r="M3" t="s"/>
-      <c r="N3" t="s"/>
-      <c r="O3" t="s"/>
-      <c r="P3" t="s"/>
-      <c r="Q3" t="s"/>
-      <c r="R3" t="s"/>
-      <c r="S3" t="s"/>
-      <c r="T3" t="s"/>
-      <c r="U3" t="s"/>
-    </row>
-    <row r="4" spans="1:21">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" t="n">
-        <v>-1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" t="s">
-        <v>69</v>
-      </c>
-      <c r="H4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" t="n">
-        <v>1</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.2696557753602469</v>
-      </c>
-      <c r="K4" t="s"/>
-      <c r="L4" t="s"/>
-      <c r="M4" t="s"/>
-      <c r="N4" t="s"/>
-      <c r="O4" t="s"/>
-      <c r="P4" t="s"/>
-      <c r="Q4" t="s"/>
-      <c r="R4" t="s"/>
-      <c r="S4" t="s"/>
-      <c r="T4" t="s"/>
-      <c r="U4" t="s"/>
-    </row>
-    <row r="5" spans="1:21">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" t="n">
-        <v>-15</v>
-      </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" t="s">
-        <v>51</v>
-      </c>
-      <c r="H5" t="n">
-        <v>1</v>
-      </c>
-      <c r="I5" t="n">
-        <v>1</v>
-      </c>
-      <c r="J5" t="n">
-        <v>14165.89734995619</v>
-      </c>
-      <c r="K5" t="s"/>
-      <c r="L5" t="s"/>
-      <c r="M5" t="s"/>
-      <c r="N5" t="s"/>
-      <c r="O5" t="s"/>
-      <c r="P5" t="s"/>
-      <c r="Q5" t="s"/>
-      <c r="R5" t="s"/>
-      <c r="S5" t="s"/>
-      <c r="T5" t="s"/>
-      <c r="U5" t="s"/>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:U4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:21">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" t="n">
-        <v>-1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" t="n">
-        <v>4</v>
-      </c>
-      <c r="I2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" t="n">
-        <v>-0.07464943567429129</v>
-      </c>
-      <c r="K2" t="s"/>
-      <c r="L2" t="n">
-        <v>1.224338557944122e-06</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0.00110649833164995</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0.7361792605749546</v>
-      </c>
-      <c r="O2" t="n">
-        <v>0.7338917975163559</v>
-      </c>
-      <c r="P2" t="s"/>
-      <c r="Q2" t="s"/>
-      <c r="R2" t="s"/>
-      <c r="S2" t="s"/>
-      <c r="T2" t="n">
-        <v>900.7836800456239</v>
-      </c>
-      <c r="U2" t="s"/>
-    </row>
-    <row r="3" spans="1:21">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>30</v>
-      </c>
-      <c r="C3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" t="n">
-        <v>-1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" t="n">
-        <v>4</v>
-      </c>
-      <c r="I3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.03641668899856448</v>
-      </c>
-      <c r="K3" t="s"/>
-      <c r="L3" t="s"/>
-      <c r="M3" t="s"/>
-      <c r="N3" t="s"/>
-      <c r="O3" t="s"/>
-      <c r="P3" t="s"/>
-      <c r="Q3" t="s"/>
-      <c r="R3" t="s"/>
-      <c r="S3" t="s"/>
-      <c r="T3" t="s"/>
-      <c r="U3" t="s"/>
-    </row>
-    <row r="4" spans="1:21">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" t="n">
-        <v>-1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" t="s">
-        <v>69</v>
-      </c>
-      <c r="H4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" t="n">
-        <v>1</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.1514673970594697</v>
-      </c>
-      <c r="K4" t="s"/>
-      <c r="L4" t="s"/>
-      <c r="M4" t="s"/>
-      <c r="N4" t="s"/>
-      <c r="O4" t="s"/>
-      <c r="P4" t="s"/>
-      <c r="Q4" t="s"/>
-      <c r="R4" t="s"/>
-      <c r="S4" t="s"/>
-      <c r="T4" t="s"/>
-      <c r="U4" t="s"/>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:U3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:21">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" t="n">
-        <v>-2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" t="s">
-        <v>77</v>
-      </c>
-      <c r="H2" t="n">
-        <v>4</v>
-      </c>
-      <c r="I2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" t="n">
-        <v>-0.01519001865908691</v>
-      </c>
-      <c r="K2" t="s"/>
-      <c r="L2" t="n">
-        <v>2.026582905942435e-06</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0.001423581014885502</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0.5633114735439935</v>
-      </c>
-      <c r="O2" t="n">
-        <v>0.5607945367920857</v>
-      </c>
-      <c r="P2" t="s"/>
-      <c r="Q2" t="s"/>
-      <c r="R2" t="s"/>
-      <c r="S2" t="s"/>
-      <c r="T2" t="n">
-        <v>1720.362459145229</v>
-      </c>
-      <c r="U2" t="s"/>
-    </row>
-    <row r="3" spans="1:21">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>30</v>
-      </c>
-      <c r="C3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" t="n">
-        <v>-1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" t="n">
-        <v>4</v>
-      </c>
-      <c r="I3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.003293821096129348</v>
-      </c>
-      <c r="K3" t="s"/>
-      <c r="L3" t="s"/>
-      <c r="M3" t="s"/>
-      <c r="N3" t="s"/>
-      <c r="O3" t="s"/>
-      <c r="P3" t="s"/>
-      <c r="Q3" t="s"/>
-      <c r="R3" t="s"/>
-      <c r="S3" t="s"/>
-      <c r="T3" t="s"/>
-      <c r="U3" t="s"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -2759,27 +2090,27 @@
         <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.1208871123618064</v>
+        <v>-0.1243688073501634</v>
       </c>
       <c r="K2" t="s"/>
       <c r="L2" t="n">
-        <v>4.014061610773389e-07</v>
+        <v>3.532759188296135e-07</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0006335662246974178</v>
+        <v>0.0005943701866931193</v>
       </c>
       <c r="N2" t="n">
-        <v>0.9135049128869912</v>
+        <v>0.9254561228294041</v>
       </c>
       <c r="O2" t="n">
-        <v>0.9098901928285371</v>
+        <v>0.9223408563207822</v>
       </c>
       <c r="P2" t="s"/>
       <c r="Q2" t="s"/>
       <c r="R2" t="s"/>
       <c r="S2" t="s"/>
       <c r="T2" t="n">
-        <v>73.1720278411475</v>
+        <v>60.5740981270873</v>
       </c>
       <c r="U2" t="s"/>
     </row>
@@ -2812,7 +2143,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="n">
-        <v>0.1290467853978869</v>
+        <v>0.07246056472963082</v>
       </c>
       <c r="K3" t="s"/>
       <c r="L3" t="s"/>
@@ -2831,31 +2162,31 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
         <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E4" t="n">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="F4" t="s">
         <v>22</v>
       </c>
       <c r="G4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I4" t="n">
         <v>1</v>
       </c>
       <c r="J4" t="n">
-        <v>-1.116953512961034</v>
+        <v>0.2089080906042933</v>
       </c>
       <c r="K4" t="s"/>
       <c r="L4" t="s"/>
@@ -2874,22 +2205,22 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
         <v>25</v>
       </c>
       <c r="E5" t="n">
-        <v>-5</v>
+        <v>-14</v>
       </c>
       <c r="F5" t="s">
         <v>22</v>
       </c>
       <c r="G5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="H5" t="n">
         <v>4</v>
@@ -2898,7 +2229,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="n">
-        <v>10.73638100892782</v>
+        <v>427738.1025750573</v>
       </c>
       <c r="K5" t="s"/>
       <c r="L5" t="s"/>
@@ -2917,22 +2248,22 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
         <v>25</v>
       </c>
       <c r="E6" t="n">
-        <v>-7</v>
+        <v>-13</v>
       </c>
       <c r="F6" t="s">
         <v>22</v>
       </c>
       <c r="G6" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="H6" t="n">
         <v>4</v>
@@ -2941,7 +2272,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="n">
-        <v>-45.01849667002372</v>
+        <v>-1004485.928011167</v>
       </c>
       <c r="K6" t="s"/>
       <c r="L6" t="s"/>
@@ -2960,22 +2291,22 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="D7" t="s">
         <v>25</v>
       </c>
       <c r="E7" t="n">
-        <v>-11</v>
+        <v>-12</v>
       </c>
       <c r="F7" t="s">
         <v>22</v>
       </c>
       <c r="G7" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="H7" t="n">
         <v>4</v>
@@ -2984,7 +2315,7 @@
         <v>1</v>
       </c>
       <c r="J7" t="n">
-        <v>734.6236442379247</v>
+        <v>940261.8233594912</v>
       </c>
       <c r="K7" t="s"/>
       <c r="L7" t="s"/>
@@ -3003,22 +2334,22 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="D8" t="s">
         <v>25</v>
       </c>
       <c r="E8" t="n">
-        <v>-12</v>
+        <v>-11</v>
       </c>
       <c r="F8" t="s">
         <v>22</v>
       </c>
       <c r="G8" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="H8" t="n">
         <v>4</v>
@@ -3027,7 +2358,7 @@
         <v>1</v>
       </c>
       <c r="J8" t="n">
-        <v>-942.431324535115</v>
+        <v>-439081.5772017264</v>
       </c>
       <c r="K8" t="s"/>
       <c r="L8" t="s"/>
@@ -3046,31 +2377,31 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="E9" t="n">
-        <v>-9</v>
+        <v>-10</v>
       </c>
       <c r="F9" t="s">
         <v>22</v>
       </c>
       <c r="G9" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="H9" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>4972430.763778246</v>
+        <v>102499.7573980587</v>
       </c>
       <c r="K9" t="s"/>
       <c r="L9" t="s"/>
@@ -3089,31 +2420,31 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="E10" t="n">
-        <v>-10</v>
+        <v>-9</v>
       </c>
       <c r="F10" t="s">
         <v>22</v>
       </c>
       <c r="G10" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="H10" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I10" t="n">
         <v>1</v>
       </c>
       <c r="J10" t="n">
-        <v>-89302524.97594878</v>
+        <v>-9600.42168018918</v>
       </c>
       <c r="K10" t="s"/>
       <c r="L10" t="s"/>
@@ -3132,22 +2463,22 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E11" t="n">
-        <v>-11</v>
+        <v>-14</v>
       </c>
       <c r="F11" t="s">
         <v>22</v>
       </c>
       <c r="G11" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="H11" t="n">
         <v>1</v>
@@ -3156,7 +2487,7 @@
         <v>1</v>
       </c>
       <c r="J11" t="n">
-        <v>675236105.9530988</v>
+        <v>480249.8447929345</v>
       </c>
       <c r="K11" t="s"/>
       <c r="L11" t="s"/>
@@ -3175,22 +2506,22 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E12" t="n">
-        <v>-12</v>
+        <v>-15</v>
       </c>
       <c r="F12" t="s">
         <v>22</v>
       </c>
       <c r="G12" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="H12" t="n">
         <v>1</v>
@@ -3199,7 +2530,7 @@
         <v>1</v>
       </c>
       <c r="J12" t="n">
-        <v>-2741031800.190311</v>
+        <v>-1005079.228785613</v>
       </c>
       <c r="K12" t="s"/>
       <c r="L12" t="s"/>
@@ -3218,22 +2549,22 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E13" t="n">
-        <v>-13</v>
+        <v>-8</v>
       </c>
       <c r="F13" t="s">
         <v>22</v>
       </c>
       <c r="G13" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="H13" t="n">
         <v>1</v>
@@ -3242,7 +2573,7 @@
         <v>1</v>
       </c>
       <c r="J13" t="n">
-        <v>6283224323.645103</v>
+        <v>-1053.220450601017</v>
       </c>
       <c r="K13" t="s"/>
       <c r="L13" t="s"/>
@@ -3261,22 +2592,22 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E14" t="n">
-        <v>-14</v>
+        <v>-7</v>
       </c>
       <c r="F14" t="s">
         <v>22</v>
       </c>
       <c r="G14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H14" t="n">
         <v>1</v>
@@ -3285,7 +2616,7 @@
         <v>1</v>
       </c>
       <c r="J14" t="n">
-        <v>-7696269616.658185</v>
+        <v>299.4448477756232</v>
       </c>
       <c r="K14" t="s"/>
       <c r="L14" t="s"/>
@@ -3304,13 +2635,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="E15" t="n">
         <v>-15</v>
@@ -3319,16 +2650,16 @@
         <v>22</v>
       </c>
       <c r="G15" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="H15" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I15" t="n">
         <v>1</v>
       </c>
       <c r="J15" t="n">
-        <v>3929840814.24644</v>
+        <v>5.463063105940819</v>
       </c>
       <c r="K15" t="s"/>
       <c r="L15" t="s"/>
@@ -3452,27 +2783,27 @@
         <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.1224898152567462</v>
+        <v>-0.1176340381873304</v>
       </c>
       <c r="K2" t="s"/>
       <c r="L2" t="n">
-        <v>4.139458221436734e-07</v>
+        <v>3.734141026955523e-07</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0006433862153820779</v>
+        <v>0.0006110761840356342</v>
       </c>
       <c r="N2" t="n">
-        <v>0.9108028639862239</v>
+        <v>0.9212068144997712</v>
       </c>
       <c r="O2" t="n">
-        <v>0.9073517843190242</v>
+        <v>0.9181582686322027</v>
       </c>
       <c r="P2" t="s"/>
       <c r="Q2" t="s"/>
       <c r="R2" t="s"/>
       <c r="S2" t="s"/>
       <c r="T2" t="n">
-        <v>84.72978677015003</v>
+        <v>81.5859180487257</v>
       </c>
       <c r="U2" t="s"/>
     </row>
@@ -3505,7 +2836,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="n">
-        <v>0.06057786024331605</v>
+        <v>0.06925156606882792</v>
       </c>
       <c r="K3" t="s"/>
       <c r="L3" t="s"/>
@@ -3524,22 +2855,22 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E4" t="n">
-        <v>-4</v>
+        <v>-1</v>
       </c>
       <c r="F4" t="s">
         <v>22</v>
       </c>
       <c r="G4" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="H4" t="n">
         <v>1</v>
@@ -3548,7 +2879,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="n">
-        <v>109.0988368594074</v>
+        <v>0.1942998716269803</v>
       </c>
       <c r="K4" t="s"/>
       <c r="L4" t="s"/>
@@ -3567,31 +2898,31 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="E5" t="n">
-        <v>-8</v>
+        <v>-14</v>
       </c>
       <c r="F5" t="s">
         <v>22</v>
       </c>
       <c r="G5" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="H5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I5" t="n">
         <v>1</v>
       </c>
       <c r="J5" t="n">
-        <v>-303276.6352682022</v>
+        <v>430750.5326265976</v>
       </c>
       <c r="K5" t="s"/>
       <c r="L5" t="s"/>
@@ -3610,31 +2941,31 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="E6" t="n">
-        <v>-10</v>
+        <v>-13</v>
       </c>
       <c r="F6" t="s">
         <v>22</v>
       </c>
       <c r="G6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H6" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I6" t="n">
         <v>1</v>
       </c>
       <c r="J6" t="n">
-        <v>26661342.75227396</v>
+        <v>-1011222.634427098</v>
       </c>
       <c r="K6" t="s"/>
       <c r="L6" t="s"/>
@@ -3653,16 +2984,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
         <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="E7" t="n">
-        <v>-11</v>
+        <v>-12</v>
       </c>
       <c r="F7" t="s">
         <v>22</v>
@@ -3671,13 +3002,13 @@
         <v>43</v>
       </c>
       <c r="H7" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I7" t="n">
         <v>1</v>
       </c>
       <c r="J7" t="n">
-        <v>-176542410.4821078</v>
+        <v>946518.5205383999</v>
       </c>
       <c r="K7" t="s"/>
       <c r="L7" t="s"/>
@@ -3696,16 +3027,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
         <v>44</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="E8" t="n">
-        <v>-12</v>
+        <v>-11</v>
       </c>
       <c r="F8" t="s">
         <v>22</v>
@@ -3714,13 +3045,13 @@
         <v>45</v>
       </c>
       <c r="H8" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I8" t="n">
         <v>1</v>
       </c>
       <c r="J8" t="n">
-        <v>477963316.8384518</v>
+        <v>-442122.4088045199</v>
       </c>
       <c r="K8" t="s"/>
       <c r="L8" t="s"/>
@@ -3739,31 +3070,31 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="E9" t="n">
-        <v>-13</v>
+        <v>-10</v>
       </c>
       <c r="F9" t="s">
         <v>22</v>
       </c>
       <c r="G9" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="H9" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>-525705724.5070662</v>
+        <v>103272.8937269928</v>
       </c>
       <c r="K9" t="s"/>
       <c r="L9" t="s"/>
@@ -3782,31 +3113,31 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="E10" t="n">
-        <v>-15</v>
+        <v>-9</v>
       </c>
       <c r="F10" t="s">
         <v>22</v>
       </c>
       <c r="G10" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="H10" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I10" t="n">
         <v>1</v>
       </c>
       <c r="J10" t="n">
-        <v>292677435.1539547</v>
+        <v>-9681.882416812017</v>
       </c>
       <c r="K10" t="s"/>
       <c r="L10" t="s"/>
@@ -3825,31 +3156,31 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E11" t="n">
-        <v>-14</v>
+        <v>-7</v>
       </c>
       <c r="F11" t="s">
         <v>22</v>
       </c>
       <c r="G11" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="H11" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I11" t="n">
         <v>1</v>
       </c>
       <c r="J11" t="n">
-        <v>-5520.336005568504</v>
+        <v>366.5851962566376</v>
       </c>
       <c r="K11" t="s"/>
       <c r="L11" t="s"/>
@@ -3868,16 +3199,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
         <v>60</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E12" t="n">
-        <v>-13</v>
+        <v>-8</v>
       </c>
       <c r="F12" t="s">
         <v>22</v>
@@ -3886,13 +3217,13 @@
         <v>61</v>
       </c>
       <c r="H12" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I12" t="n">
         <v>1</v>
       </c>
       <c r="J12" t="n">
-        <v>7548.2493250072</v>
+        <v>-1387.923360378481</v>
       </c>
       <c r="K12" t="s"/>
       <c r="L12" t="s"/>
@@ -3911,13 +3242,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E13" t="n">
         <v>-12</v>
@@ -3926,16 +3257,16 @@
         <v>22</v>
       </c>
       <c r="G13" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="H13" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I13" t="n">
         <v>1</v>
       </c>
       <c r="J13" t="n">
-        <v>-3327.420893967152</v>
+        <v>43514.28051067487</v>
       </c>
       <c r="K13" t="s"/>
       <c r="L13" t="s"/>
@@ -3954,31 +3285,31 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D14" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E14" t="n">
-        <v>-11</v>
+        <v>-14</v>
       </c>
       <c r="F14" t="s">
         <v>22</v>
       </c>
       <c r="G14" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="H14" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I14" t="n">
         <v>1</v>
       </c>
       <c r="J14" t="n">
-        <v>465.7295291423798</v>
+        <v>-148796.8860814089</v>
       </c>
       <c r="K14" t="s"/>
       <c r="L14" t="s"/>
@@ -4102,27 +3433,27 @@
         <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.1229528130347403</v>
+        <v>-0.1184019768709303</v>
       </c>
       <c r="K2" t="s"/>
       <c r="L2" t="n">
-        <v>4.14324811153034e-07</v>
+        <v>3.762068346457605e-07</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0006436806748326642</v>
+        <v>0.0006133570205400444</v>
       </c>
       <c r="N2" t="n">
-        <v>0.9107211993518507</v>
+        <v>0.9206175270437894</v>
       </c>
       <c r="O2" t="n">
-        <v>0.9075421322664566</v>
+        <v>0.9177908514489095</v>
       </c>
       <c r="P2" t="s"/>
       <c r="Q2" t="s"/>
       <c r="R2" t="s"/>
       <c r="S2" t="s"/>
       <c r="T2" t="n">
-        <v>84.3179586844802</v>
+        <v>83.83178029835635</v>
       </c>
       <c r="U2" t="s"/>
     </row>
@@ -4155,7 +3486,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="n">
-        <v>0.06120134138244926</v>
+        <v>0.06959851994685147</v>
       </c>
       <c r="K3" t="s"/>
       <c r="L3" t="s"/>
@@ -4174,22 +3505,22 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E4" t="n">
-        <v>-4</v>
+        <v>-1</v>
       </c>
       <c r="F4" t="s">
         <v>22</v>
       </c>
       <c r="G4" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="H4" t="n">
         <v>1</v>
@@ -4198,7 +3529,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="n">
-        <v>108.6854819944018</v>
+        <v>0.1868071392050911</v>
       </c>
       <c r="K4" t="s"/>
       <c r="L4" t="s"/>
@@ -4217,22 +3548,22 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E5" t="n">
-        <v>-8</v>
+        <v>-7</v>
       </c>
       <c r="F5" t="s">
         <v>22</v>
       </c>
       <c r="G5" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="H5" t="n">
         <v>1</v>
@@ -4241,7 +3572,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="n">
-        <v>-301971.6049426379</v>
+        <v>294.5629589023249</v>
       </c>
       <c r="K5" t="s"/>
       <c r="L5" t="s"/>
@@ -4260,22 +3591,22 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E6" t="n">
-        <v>-10</v>
+        <v>-6</v>
       </c>
       <c r="F6" t="s">
         <v>22</v>
       </c>
       <c r="G6" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="H6" t="n">
         <v>1</v>
@@ -4284,7 +3615,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="n">
-        <v>26549028.37717194</v>
+        <v>-210.1267461966937</v>
       </c>
       <c r="K6" t="s"/>
       <c r="L6" t="s"/>
@@ -4303,22 +3634,22 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E7" t="n">
-        <v>-11</v>
+        <v>-5</v>
       </c>
       <c r="F7" t="s">
         <v>22</v>
       </c>
       <c r="G7" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="H7" t="n">
         <v>1</v>
@@ -4327,7 +3658,7 @@
         <v>1</v>
       </c>
       <c r="J7" t="n">
-        <v>-175812665.7323788</v>
+        <v>39.76144792950228</v>
       </c>
       <c r="K7" t="s"/>
       <c r="L7" t="s"/>
@@ -4346,31 +3677,31 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="E8" t="n">
-        <v>-12</v>
+        <v>-14</v>
       </c>
       <c r="F8" t="s">
         <v>22</v>
       </c>
       <c r="G8" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="H8" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I8" t="n">
         <v>1</v>
       </c>
       <c r="J8" t="n">
-        <v>476033377.0385846</v>
+        <v>430323.5701968353</v>
       </c>
       <c r="K8" t="s"/>
       <c r="L8" t="s"/>
@@ -4389,13 +3720,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="E9" t="n">
         <v>-13</v>
@@ -4404,16 +3735,16 @@
         <v>22</v>
       </c>
       <c r="G9" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="H9" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>-523640311.6294076</v>
+        <v>-1009250.886480522</v>
       </c>
       <c r="K9" t="s"/>
       <c r="L9" t="s"/>
@@ -4432,31 +3763,31 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="E10" t="n">
-        <v>-15</v>
+        <v>-12</v>
       </c>
       <c r="F10" t="s">
         <v>22</v>
       </c>
       <c r="G10" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="H10" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I10" t="n">
         <v>1</v>
       </c>
       <c r="J10" t="n">
-        <v>291599958.5611746</v>
+        <v>943699.1179453006</v>
       </c>
       <c r="K10" t="s"/>
       <c r="L10" t="s"/>
@@ -4475,22 +3806,22 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="D11" t="s">
         <v>25</v>
       </c>
       <c r="E11" t="n">
-        <v>-13</v>
+        <v>-11</v>
       </c>
       <c r="F11" t="s">
         <v>22</v>
       </c>
       <c r="G11" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="H11" t="n">
         <v>4</v>
@@ -4499,7 +3830,7 @@
         <v>1</v>
       </c>
       <c r="J11" t="n">
-        <v>-1292.006356775761</v>
+        <v>-440321.8627108715</v>
       </c>
       <c r="K11" t="s"/>
       <c r="L11" t="s"/>
@@ -4518,22 +3849,22 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D12" t="s">
         <v>25</v>
       </c>
       <c r="E12" t="n">
-        <v>-14</v>
+        <v>-10</v>
       </c>
       <c r="F12" t="s">
         <v>22</v>
       </c>
       <c r="G12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H12" t="n">
         <v>4</v>
@@ -4542,7 +3873,7 @@
         <v>1</v>
       </c>
       <c r="J12" t="n">
-        <v>4798.773107469082</v>
+        <v>102734.8972289835</v>
       </c>
       <c r="K12" t="s"/>
       <c r="L12" t="s"/>
@@ -4561,22 +3892,22 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D13" t="s">
         <v>25</v>
       </c>
       <c r="E13" t="n">
-        <v>-15</v>
+        <v>-9</v>
       </c>
       <c r="F13" t="s">
         <v>22</v>
       </c>
       <c r="G13" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H13" t="n">
         <v>4</v>
@@ -4585,7 +3916,7 @@
         <v>1</v>
       </c>
       <c r="J13" t="n">
-        <v>-4449.448174715042</v>
+        <v>-9620.511388322804</v>
       </c>
       <c r="K13" t="s"/>
       <c r="L13" t="s"/>
@@ -4685,13 +4016,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E2" t="n">
         <v>-1</v>
@@ -4700,7 +4031,7 @@
         <v>22</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H2" t="n">
         <v>4</v>
@@ -4709,27 +4040,27 @@
         <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.1229143120093299</v>
+        <v>0.06388428100960861</v>
       </c>
       <c r="K2" t="s"/>
       <c r="L2" t="n">
-        <v>4.236925048106682e-07</v>
+        <v>3.7409265233878e-07</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0006509166650276117</v>
+        <v>0.0006116311407529704</v>
       </c>
       <c r="N2" t="n">
-        <v>0.9087026466799376</v>
+        <v>0.9210636354191634</v>
       </c>
       <c r="O2" t="n">
-        <v>0.9057314310393438</v>
+        <v>0.9184947004771835</v>
       </c>
       <c r="P2" t="s"/>
       <c r="Q2" t="s"/>
       <c r="R2" t="s"/>
       <c r="S2" t="s"/>
       <c r="T2" t="n">
-        <v>92.83646474910638</v>
+        <v>80.73434076391996</v>
       </c>
       <c r="U2" t="s"/>
     </row>
@@ -4738,31 +4069,31 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="E3" t="n">
-        <v>-4</v>
+        <v>-1</v>
       </c>
       <c r="F3" t="s">
         <v>22</v>
       </c>
       <c r="G3" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="H3" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I3" t="n">
         <v>1</v>
       </c>
       <c r="J3" t="n">
-        <v>86.52996300304468</v>
+        <v>-0.1247006137387482</v>
       </c>
       <c r="K3" t="s"/>
       <c r="L3" t="s"/>
@@ -4781,13 +4112,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E4" t="n">
         <v>-1</v>
@@ -4796,16 +4127,16 @@
         <v>22</v>
       </c>
       <c r="G4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I4" t="n">
         <v>1</v>
       </c>
       <c r="J4" t="n">
-        <v>0.07032725963462383</v>
+        <v>0.2445686082596114</v>
       </c>
       <c r="K4" t="s"/>
       <c r="L4" t="s"/>
@@ -4824,22 +4155,22 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E5" t="n">
-        <v>-9</v>
+        <v>-12</v>
       </c>
       <c r="F5" t="s">
         <v>22</v>
       </c>
       <c r="G5" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="H5" t="n">
         <v>1</v>
@@ -4848,7 +4179,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="n">
-        <v>-3744374.246021292</v>
+        <v>781.4929266570352</v>
       </c>
       <c r="K5" t="s"/>
       <c r="L5" t="s"/>
@@ -4867,31 +4198,31 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="E6" t="n">
-        <v>-10</v>
+        <v>-15</v>
       </c>
       <c r="F6" t="s">
         <v>22</v>
       </c>
       <c r="G6" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="H6" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I6" t="n">
         <v>1</v>
       </c>
       <c r="J6" t="n">
-        <v>43205703.62871289</v>
+        <v>4.215374075728035</v>
       </c>
       <c r="K6" t="s"/>
       <c r="L6" t="s"/>
@@ -4910,31 +4241,31 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="E7" t="n">
-        <v>-11</v>
+        <v>-15</v>
       </c>
       <c r="F7" t="s">
         <v>22</v>
       </c>
       <c r="G7" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="H7" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I7" t="n">
         <v>1</v>
       </c>
       <c r="J7" t="n">
-        <v>-190665517.0656868</v>
+        <v>546907.490111545</v>
       </c>
       <c r="K7" t="s"/>
       <c r="L7" t="s"/>
@@ -4953,31 +4284,31 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="E8" t="n">
-        <v>-12</v>
+        <v>-14</v>
       </c>
       <c r="F8" t="s">
         <v>22</v>
       </c>
       <c r="G8" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="H8" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I8" t="n">
         <v>1</v>
       </c>
       <c r="J8" t="n">
-        <v>344130921.3013142</v>
+        <v>-1245568.466406116</v>
       </c>
       <c r="K8" t="s"/>
       <c r="L8" t="s"/>
@@ -4996,31 +4327,31 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="E9" t="n">
-        <v>-14</v>
+        <v>-13</v>
       </c>
       <c r="F9" t="s">
         <v>22</v>
       </c>
       <c r="G9" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="H9" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>-789896502.702287</v>
+        <v>1125382.135864628</v>
       </c>
       <c r="K9" t="s"/>
       <c r="L9" t="s"/>
@@ -5039,31 +4370,31 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="E10" t="n">
-        <v>-15</v>
+        <v>-12</v>
       </c>
       <c r="F10" t="s">
         <v>22</v>
       </c>
       <c r="G10" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="H10" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I10" t="n">
         <v>1</v>
       </c>
       <c r="J10" t="n">
-        <v>738501708.6890553</v>
+        <v>-504499.422205847</v>
       </c>
       <c r="K10" t="s"/>
       <c r="L10" t="s"/>
@@ -5085,7 +4416,7 @@
         <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="D11" t="s">
         <v>25</v>
@@ -5097,7 +4428,7 @@
         <v>22</v>
       </c>
       <c r="G11" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="H11" t="n">
         <v>4</v>
@@ -5106,7 +4437,7 @@
         <v>1</v>
       </c>
       <c r="J11" t="n">
-        <v>1.610732450695615</v>
+        <v>112378.2480822044</v>
       </c>
       <c r="K11" t="s"/>
       <c r="L11" t="s"/>
@@ -5125,22 +4456,22 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="D12" t="s">
         <v>25</v>
       </c>
       <c r="E12" t="n">
-        <v>-2</v>
+        <v>-10</v>
       </c>
       <c r="F12" t="s">
         <v>22</v>
       </c>
       <c r="G12" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="H12" t="n">
         <v>4</v>
@@ -5149,7 +4480,7 @@
         <v>1</v>
       </c>
       <c r="J12" t="n">
-        <v>-0.01981004871767311</v>
+        <v>-9980.646503983118</v>
       </c>
       <c r="K12" t="s"/>
       <c r="L12" t="s"/>
@@ -5249,13 +4580,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E2" t="n">
         <v>-1</v>
@@ -5264,7 +4595,7 @@
         <v>22</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H2" t="n">
         <v>4</v>
@@ -5273,27 +4604,27 @@
         <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.1191713084516842</v>
+        <v>0.06351684635296498</v>
       </c>
       <c r="K2" t="s"/>
       <c r="L2" t="n">
-        <v>4.374791002185886e-07</v>
+        <v>3.880697209840752e-07</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0006614220288277286</v>
+        <v>0.000622952422729116</v>
       </c>
       <c r="N2" t="n">
-        <v>0.9057319080953594</v>
+        <v>0.918114368761669</v>
       </c>
       <c r="O2" t="n">
-        <v>0.9029511384226562</v>
+        <v>0.9156988634154055</v>
       </c>
       <c r="P2" t="s"/>
       <c r="Q2" t="s"/>
       <c r="R2" t="s"/>
       <c r="S2" t="s"/>
       <c r="T2" t="n">
-        <v>105.8119268161041</v>
+        <v>95.25646676307284</v>
       </c>
       <c r="U2" t="s"/>
     </row>
@@ -5302,13 +4633,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E3" t="n">
         <v>-1</v>
@@ -5317,7 +4648,7 @@
         <v>22</v>
       </c>
       <c r="G3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H3" t="n">
         <v>4</v>
@@ -5326,7 +4657,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="n">
-        <v>0.05814171829611445</v>
+        <v>-0.1262262779706325</v>
       </c>
       <c r="K3" t="s"/>
       <c r="L3" t="s"/>
@@ -5345,22 +4676,22 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E4" t="n">
-        <v>-4</v>
+        <v>-1</v>
       </c>
       <c r="F4" t="s">
         <v>22</v>
       </c>
       <c r="G4" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="H4" t="n">
         <v>1</v>
@@ -5369,7 +4700,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="n">
-        <v>112.7303029829309</v>
+        <v>0.2501387497068529</v>
       </c>
       <c r="K4" t="s"/>
       <c r="L4" t="s"/>
@@ -5388,22 +4719,22 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E5" t="n">
-        <v>-7</v>
+        <v>-13</v>
       </c>
       <c r="F5" t="s">
         <v>22</v>
       </c>
       <c r="G5" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="H5" t="n">
         <v>1</v>
@@ -5412,7 +4743,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="n">
-        <v>-24821.36900931638</v>
+        <v>2039.757683622538</v>
       </c>
       <c r="K5" t="s"/>
       <c r="L5" t="s"/>
@@ -5431,31 +4762,31 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="E6" t="n">
-        <v>-10</v>
+        <v>-13</v>
       </c>
       <c r="F6" t="s">
         <v>22</v>
       </c>
       <c r="G6" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="H6" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I6" t="n">
         <v>1</v>
       </c>
       <c r="J6" t="n">
-        <v>4972591.873205935</v>
+        <v>1.431123206961792</v>
       </c>
       <c r="K6" t="s"/>
       <c r="L6" t="s"/>
@@ -5474,31 +4805,31 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="E7" t="n">
-        <v>-12</v>
+        <v>-15</v>
       </c>
       <c r="F7" t="s">
         <v>22</v>
       </c>
       <c r="G7" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="H7" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I7" t="n">
         <v>1</v>
       </c>
       <c r="J7" t="n">
-        <v>-214542046.92409</v>
+        <v>77926.27442651289</v>
       </c>
       <c r="K7" t="s"/>
       <c r="L7" t="s"/>
@@ -5517,31 +4848,31 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="E8" t="n">
-        <v>-13</v>
+        <v>-14</v>
       </c>
       <c r="F8" t="s">
         <v>22</v>
       </c>
       <c r="G8" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="H8" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I8" t="n">
         <v>1</v>
       </c>
       <c r="J8" t="n">
-        <v>984454545.3075018</v>
+        <v>-146755.5999379722</v>
       </c>
       <c r="K8" t="s"/>
       <c r="L8" t="s"/>
@@ -5560,31 +4891,31 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="E9" t="n">
-        <v>-14</v>
+        <v>-13</v>
       </c>
       <c r="F9" t="s">
         <v>22</v>
       </c>
       <c r="G9" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="H9" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>-1761778402.28189</v>
+        <v>101717.7267437129</v>
       </c>
       <c r="K9" t="s"/>
       <c r="L9" t="s"/>
@@ -5603,31 +4934,31 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="E10" t="n">
-        <v>-15</v>
+        <v>-12</v>
       </c>
       <c r="F10" t="s">
         <v>22</v>
       </c>
       <c r="G10" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="H10" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I10" t="n">
         <v>1</v>
       </c>
       <c r="J10" t="n">
-        <v>1153559094.304512</v>
+        <v>-30551.63241214858</v>
       </c>
       <c r="K10" t="s"/>
       <c r="L10" t="s"/>
@@ -5646,22 +4977,22 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
         <v>44</v>
-      </c>
-      <c r="C11" t="s">
-        <v>62</v>
       </c>
       <c r="D11" t="s">
         <v>25</v>
       </c>
       <c r="E11" t="n">
-        <v>-15</v>
+        <v>-11</v>
       </c>
       <c r="F11" t="s">
         <v>22</v>
       </c>
       <c r="G11" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="H11" t="n">
         <v>4</v>
@@ -5670,7 +5001,7 @@
         <v>1</v>
       </c>
       <c r="J11" t="n">
-        <v>5.74591110669275</v>
+        <v>3319.250088446101</v>
       </c>
       <c r="K11" t="s"/>
       <c r="L11" t="s"/>
@@ -5770,13 +5101,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E2" t="n">
         <v>-1</v>
@@ -5785,7 +5116,7 @@
         <v>22</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H2" t="n">
         <v>4</v>
@@ -5794,27 +5125,27 @@
         <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.1209833930364427</v>
+        <v>0.06476507896195886</v>
       </c>
       <c r="K2" t="s"/>
       <c r="L2" t="n">
-        <v>4.428978757100064e-07</v>
+        <v>3.936234255478975e-07</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0006655057292841336</v>
+        <v>0.0006273941548563371</v>
       </c>
       <c r="N2" t="n">
-        <v>0.9045642691709391</v>
+        <v>0.9169424953087065</v>
       </c>
       <c r="O2" t="n">
-        <v>0.9020380292372286</v>
+        <v>0.9147439143021723</v>
       </c>
       <c r="P2" t="s"/>
       <c r="Q2" t="s"/>
       <c r="R2" t="s"/>
       <c r="S2" t="s"/>
       <c r="T2" t="n">
-        <v>110.5077287142697</v>
+        <v>100.6110085464891</v>
       </c>
       <c r="U2" t="s"/>
     </row>
@@ -5823,13 +5154,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E3" t="n">
         <v>-1</v>
@@ -5838,7 +5169,7 @@
         <v>22</v>
       </c>
       <c r="G3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H3" t="n">
         <v>4</v>
@@ -5847,7 +5178,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="n">
-        <v>0.05927185289776223</v>
+        <v>-0.1271243483506609</v>
       </c>
       <c r="K3" t="s"/>
       <c r="L3" t="s"/>
@@ -5866,22 +5197,22 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E4" t="n">
-        <v>-4</v>
+        <v>-1</v>
       </c>
       <c r="F4" t="s">
         <v>22</v>
       </c>
       <c r="G4" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="H4" t="n">
         <v>1</v>
@@ -5890,7 +5221,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="n">
-        <v>113.8298889035877</v>
+        <v>0.2494110089713984</v>
       </c>
       <c r="K4" t="s"/>
       <c r="L4" t="s"/>
@@ -5909,22 +5240,22 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E5" t="n">
-        <v>-7</v>
+        <v>-12</v>
       </c>
       <c r="F5" t="s">
         <v>22</v>
       </c>
       <c r="G5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H5" t="n">
         <v>1</v>
@@ -5933,7 +5264,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="n">
-        <v>-25037.82718642418</v>
+        <v>818.65181771871</v>
       </c>
       <c r="K5" t="s"/>
       <c r="L5" t="s"/>
@@ -5952,31 +5283,31 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="E6" t="n">
-        <v>-10</v>
+        <v>-12</v>
       </c>
       <c r="F6" t="s">
         <v>22</v>
       </c>
       <c r="G6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="H6" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I6" t="n">
         <v>1</v>
       </c>
       <c r="J6" t="n">
-        <v>5012404.277860065</v>
+        <v>-3125.516497455135</v>
       </c>
       <c r="K6" t="s"/>
       <c r="L6" t="s"/>
@@ -5995,31 +5326,31 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="E7" t="n">
-        <v>-12</v>
+        <v>-13</v>
       </c>
       <c r="F7" t="s">
         <v>22</v>
       </c>
       <c r="G7" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="H7" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I7" t="n">
         <v>1</v>
       </c>
       <c r="J7" t="n">
-        <v>-216186643.2967186</v>
+        <v>17026.14966150884</v>
       </c>
       <c r="K7" t="s"/>
       <c r="L7" t="s"/>
@@ -6038,31 +5369,31 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="E8" t="n">
-        <v>-13</v>
+        <v>-14</v>
       </c>
       <c r="F8" t="s">
         <v>22</v>
       </c>
       <c r="G8" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="H8" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I8" t="n">
         <v>1</v>
       </c>
       <c r="J8" t="n">
-        <v>991863800.0185891</v>
+        <v>-30958.79864279469</v>
       </c>
       <c r="K8" t="s"/>
       <c r="L8" t="s"/>
@@ -6081,31 +5412,31 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="E9" t="n">
-        <v>-14</v>
+        <v>-15</v>
       </c>
       <c r="F9" t="s">
         <v>22</v>
       </c>
       <c r="G9" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="H9" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>-1774818093.075379</v>
+        <v>3.738244080108718</v>
       </c>
       <c r="K9" t="s"/>
       <c r="L9" t="s"/>
@@ -6124,13 +5455,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="E10" t="n">
         <v>-15</v>
@@ -6139,16 +5470,16 @@
         <v>22</v>
       </c>
       <c r="G10" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="H10" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I10" t="n">
         <v>1</v>
       </c>
       <c r="J10" t="n">
-        <v>1161964653.865471</v>
+        <v>18787.37583560703</v>
       </c>
       <c r="K10" t="s"/>
       <c r="L10" t="s"/>
@@ -6248,13 +5579,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E2" t="n">
         <v>-1</v>
@@ -6263,7 +5594,7 @@
         <v>22</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H2" t="n">
         <v>4</v>
@@ -6272,27 +5603,27 @@
         <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.1219746759699044</v>
+        <v>0.06469163257643816</v>
       </c>
       <c r="K2" t="s"/>
       <c r="L2" t="n">
-        <v>4.537848026101771e-07</v>
+        <v>4.006686848124171e-07</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0006736355116902442</v>
+        <v>0.0006329839530449545</v>
       </c>
       <c r="N2" t="n">
-        <v>0.9022183517886651</v>
+        <v>0.9154558925903857</v>
       </c>
       <c r="O2" t="n">
-        <v>0.8999243541766689</v>
+        <v>0.9134724531203655</v>
       </c>
       <c r="P2" t="s"/>
       <c r="Q2" t="s"/>
       <c r="R2" t="s"/>
       <c r="S2" t="s"/>
       <c r="T2" t="n">
-        <v>120.7146403351184</v>
+        <v>107.6454470690431</v>
       </c>
       <c r="U2" t="s"/>
     </row>
@@ -6301,13 +5632,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="E3" t="n">
         <v>-1</v>
@@ -6316,16 +5647,16 @@
         <v>22</v>
       </c>
       <c r="G3" t="s">
-        <v>69</v>
+        <v>23</v>
       </c>
       <c r="H3" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I3" t="n">
         <v>1</v>
       </c>
       <c r="J3" t="n">
-        <v>0.2448201856852009</v>
+        <v>-0.1268447439170436</v>
       </c>
       <c r="K3" t="s"/>
       <c r="L3" t="s"/>
@@ -6344,13 +5675,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E4" t="n">
         <v>-1</v>
@@ -6359,16 +5690,16 @@
         <v>22</v>
       </c>
       <c r="G4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I4" t="n">
         <v>1</v>
       </c>
       <c r="J4" t="n">
-        <v>0.06085137027160281</v>
+        <v>0.2488203322929143</v>
       </c>
       <c r="K4" t="s"/>
       <c r="L4" t="s"/>
@@ -6387,22 +5718,22 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E5" t="n">
-        <v>-13</v>
+        <v>-12</v>
       </c>
       <c r="F5" t="s">
         <v>22</v>
       </c>
       <c r="G5" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="H5" t="n">
         <v>1</v>
@@ -6411,7 +5742,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="n">
-        <v>3699.632475950687</v>
+        <v>801.8440385931574</v>
       </c>
       <c r="K5" t="s"/>
       <c r="L5" t="s"/>
@@ -6430,31 +5761,31 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="E6" t="n">
-        <v>-6</v>
+        <v>-8</v>
       </c>
       <c r="F6" t="s">
         <v>22</v>
       </c>
       <c r="G6" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="H6" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I6" t="n">
         <v>1</v>
       </c>
       <c r="J6" t="n">
-        <v>-1.503287200999365</v>
+        <v>-3.925922295554146</v>
       </c>
       <c r="K6" t="s"/>
       <c r="L6" t="s"/>
@@ -6473,22 +5804,22 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
         <v>42</v>
-      </c>
-      <c r="C7" t="s">
-        <v>60</v>
       </c>
       <c r="D7" t="s">
         <v>25</v>
       </c>
       <c r="E7" t="n">
-        <v>-13</v>
+        <v>-12</v>
       </c>
       <c r="F7" t="s">
         <v>22</v>
       </c>
       <c r="G7" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="H7" t="n">
         <v>4</v>
@@ -6497,7 +5828,7 @@
         <v>1</v>
       </c>
       <c r="J7" t="n">
-        <v>-1385.868604604526</v>
+        <v>218.3081548567692</v>
       </c>
       <c r="K7" t="s"/>
       <c r="L7" t="s"/>
@@ -6516,22 +5847,22 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
         <v>25</v>
       </c>
       <c r="E8" t="n">
-        <v>-14</v>
+        <v>-13</v>
       </c>
       <c r="F8" t="s">
         <v>22</v>
       </c>
       <c r="G8" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="H8" t="n">
         <v>4</v>
@@ -6540,7 +5871,7 @@
         <v>1</v>
       </c>
       <c r="J8" t="n">
-        <v>5111.995629554719</v>
+        <v>-319.2082917540949</v>
       </c>
       <c r="K8" t="s"/>
       <c r="L8" t="s"/>
@@ -6559,13 +5890,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
         <v>62</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E9" t="n">
         <v>-15</v>
@@ -6583,7 +5914,7 @@
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>-4708.348573907367</v>
+        <v>3.943094924749631</v>
       </c>
       <c r="K9" t="s"/>
       <c r="L9" t="s"/>
@@ -6707,27 +6038,27 @@
         <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>0.06300357457802004</v>
+        <v>0.06216247479544443</v>
       </c>
       <c r="K2" t="s"/>
       <c r="L2" t="n">
-        <v>4.612244455121389e-07</v>
+        <v>4.143124740507617e-07</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0006791350716257694</v>
+        <v>0.0006436710915139514</v>
       </c>
       <c r="N2" t="n">
-        <v>0.9006152559139835</v>
+        <v>0.9125769503955876</v>
       </c>
       <c r="O2" t="n">
-        <v>0.8985810652455563</v>
+        <v>0.9107875897311698</v>
       </c>
       <c r="P2" t="s"/>
       <c r="Q2" t="s"/>
       <c r="R2" t="s"/>
       <c r="S2" t="s"/>
       <c r="T2" t="n">
-        <v>127.5209004886296</v>
+        <v>122.0199345178706</v>
       </c>
       <c r="U2" t="s"/>
     </row>
@@ -6760,7 +6091,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="n">
-        <v>-0.1237024210201753</v>
+        <v>-0.1222426032191814</v>
       </c>
       <c r="K3" t="s"/>
       <c r="L3" t="s"/>
@@ -6782,10 +6113,10 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E4" t="n">
         <v>-1</v>
@@ -6794,7 +6125,7 @@
         <v>22</v>
       </c>
       <c r="G4" t="s">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="H4" t="n">
         <v>1</v>
@@ -6803,7 +6134,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="n">
-        <v>0.242625355919287</v>
+        <v>0.2405189306662942</v>
       </c>
       <c r="K4" t="s"/>
       <c r="L4" t="s"/>
@@ -6825,10 +6156,10 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E5" t="n">
         <v>-15</v>
@@ -6837,7 +6168,7 @@
         <v>22</v>
       </c>
       <c r="G5" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="H5" t="n">
         <v>1</v>
@@ -6846,7 +6177,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="n">
-        <v>19328.4772706353</v>
+        <v>16916.54437455959</v>
       </c>
       <c r="K5" t="s"/>
       <c r="L5" t="s"/>
@@ -6868,7 +6199,7 @@
         <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D6" t="s">
         <v>25</v>
@@ -6880,7 +6211,7 @@
         <v>22</v>
       </c>
       <c r="G6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H6" t="n">
         <v>4</v>
@@ -6889,7 +6220,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="n">
-        <v>-2.536747642392877</v>
+        <v>-3.628125902615099</v>
       </c>
       <c r="K6" t="s"/>
       <c r="L6" t="s"/>
@@ -6908,22 +6239,22 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="D7" t="s">
         <v>25</v>
       </c>
       <c r="E7" t="n">
-        <v>-14</v>
+        <v>-12</v>
       </c>
       <c r="F7" t="s">
         <v>22</v>
       </c>
       <c r="G7" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="H7" t="n">
         <v>4</v>
@@ -6932,7 +6263,7 @@
         <v>1</v>
       </c>
       <c r="J7" t="n">
-        <v>634.3398985270418</v>
+        <v>205.0235428143337</v>
       </c>
       <c r="K7" t="s"/>
       <c r="L7" t="s"/>
@@ -6951,22 +6282,22 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
         <v>25</v>
       </c>
       <c r="E8" t="n">
-        <v>-15</v>
+        <v>-13</v>
       </c>
       <c r="F8" t="s">
         <v>22</v>
       </c>
       <c r="G8" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="H8" t="n">
         <v>4</v>
@@ -6975,7 +6306,7 @@
         <v>1</v>
       </c>
       <c r="J8" t="n">
-        <v>-986.98306017298</v>
+        <v>-300.5112814814161</v>
       </c>
       <c r="K8" t="s"/>
       <c r="L8" t="s"/>

</xml_diff>